<commit_message>
Add also at to by institute author list
</commit_message>
<xml_diff>
--- a/11-CollaborationList/Imperial.xlsx
+++ b/11-CollaborationList/Imperial.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/longkr/KL-GIT/CCAP/02-LhARA/00-Collaboration-lists/11-CollaborationList/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/00-Collaboration-lists/11-CollaborationList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B9B976-695A-9B40-AC62-82F5C1A3F1B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F033F06D-ED9A-C949-965F-086E49C74744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="0" windowWidth="28040" windowHeight="17440" xr2:uid="{7B5F04B9-63DF-474E-BF2F-8D8D82A0D772}"/>
+    <workbookView xWindow="2200" yWindow="640" windowWidth="28040" windowHeight="17440" xr2:uid="{7B5F04B9-63DF-474E-BF2F-8D8D82A0D772}"/>
   </bookViews>
   <sheets>
     <sheet name="Imperial" sheetId="1" r:id="rId1"/>
@@ -1378,8 +1378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C3A07F-0925-B14D-9B78-C81CB9121297}">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1813,7 +1813,7 @@
         <v>152</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J12" t="s">
         <v>89</v>
@@ -1886,7 +1886,7 @@
         <v>152</v>
       </c>
       <c r="I14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J14" t="s">
         <v>89</v>
@@ -1965,7 +1965,7 @@
         <v>152</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J16" t="s">
         <v>89</v>
@@ -2076,7 +2076,7 @@
         <v>152</v>
       </c>
       <c r="I19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J19" t="s">
         <v>89</v>
@@ -2158,7 +2158,7 @@
         <v>152</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J21" t="s">
         <v>89</v>

</xml_diff>